<commit_message>
gift for new player
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Item.xlsx
+++ b/_Out/NFDataCfg/Excel/Item.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="23360"/>
+    <workbookView windowWidth="18405" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Property_scrolls-3-building" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="592">
   <si>
     <t>Id</t>
   </si>
@@ -206,7 +206,7 @@
     <t>UIResources/BuilderSprite</t>
   </si>
   <si>
-    <t>NameID_Item_Building000</t>
+    <t>NameID_Building000</t>
   </si>
   <si>
     <t>Item_Building001</t>
@@ -218,7 +218,7 @@
     <t>Building001</t>
   </si>
   <si>
-    <t>NameID_Item_Building001</t>
+    <t>NameID_Building001</t>
   </si>
   <si>
     <t>Item_Building002</t>
@@ -230,7 +230,7 @@
     <t>Building002</t>
   </si>
   <si>
-    <t>NameID_Item_Building002</t>
+    <t>NameID_Building002</t>
   </si>
   <si>
     <t>Item_Building010</t>
@@ -242,7 +242,7 @@
     <t>Building010</t>
   </si>
   <si>
-    <t>NameID_Item_Building010</t>
+    <t>NameID_Building010</t>
   </si>
   <si>
     <t>Item_Building011</t>
@@ -254,7 +254,7 @@
     <t>Building011</t>
   </si>
   <si>
-    <t>NameID_Item_Building011</t>
+    <t>NameID_Building011</t>
   </si>
   <si>
     <t>Item_Building012</t>
@@ -266,7 +266,7 @@
     <t>Building012</t>
   </si>
   <si>
-    <t>NameID_Item_Building012</t>
+    <t>NameID_Building012</t>
   </si>
   <si>
     <t>Item_Building020</t>
@@ -278,7 +278,7 @@
     <t>Building020</t>
   </si>
   <si>
-    <t>NameID_Item_Building020</t>
+    <t>NameID_Building020</t>
   </si>
   <si>
     <t>Item_Building021</t>
@@ -290,7 +290,7 @@
     <t>Building021</t>
   </si>
   <si>
-    <t>NameID_Item_Building021</t>
+    <t>NameID_Building021</t>
   </si>
   <si>
     <t>Item_Building022</t>
@@ -302,7 +302,7 @@
     <t>Building022</t>
   </si>
   <si>
-    <t>NameID_Item_Building022</t>
+    <t>NameID_Building022</t>
   </si>
   <si>
     <t>Item_Building030</t>
@@ -314,7 +314,7 @@
     <t>Building030</t>
   </si>
   <si>
-    <t>NameID_Item_Building030</t>
+    <t>NameID_Building030</t>
   </si>
   <si>
     <t>Item_Building031</t>
@@ -326,7 +326,7 @@
     <t>Building031</t>
   </si>
   <si>
-    <t>NameID_Item_Building031</t>
+    <t>NameID_Building031</t>
   </si>
   <si>
     <t>Item_Building032</t>
@@ -338,7 +338,7 @@
     <t>Building032</t>
   </si>
   <si>
-    <t>NameID_Item_Building032</t>
+    <t>NameID_Building032</t>
   </si>
   <si>
     <t>Item_Building040</t>
@@ -350,7 +350,7 @@
     <t>Building040</t>
   </si>
   <si>
-    <t>NameID_Item_Building040</t>
+    <t>NameID_Building040</t>
   </si>
   <si>
     <t>Item_Building041</t>
@@ -362,7 +362,7 @@
     <t>Building041</t>
   </si>
   <si>
-    <t>NameID_Item_Building041</t>
+    <t>NameID_Building041</t>
   </si>
   <si>
     <t>Item_Building042</t>
@@ -374,7 +374,7 @@
     <t>Building042</t>
   </si>
   <si>
-    <t>NameID_Item_Building042</t>
+    <t>NameID_Building042</t>
   </si>
   <si>
     <t>Item_Building050</t>
@@ -386,7 +386,7 @@
     <t>Building050</t>
   </si>
   <si>
-    <t>NameID_Item_Building050</t>
+    <t>NameID_Building050</t>
   </si>
   <si>
     <t>Item_Building051</t>
@@ -398,7 +398,7 @@
     <t>Building051</t>
   </si>
   <si>
-    <t>NameID_Item_Building051</t>
+    <t>NameID_Building051</t>
   </si>
   <si>
     <t>Item_Building052</t>
@@ -410,7 +410,7 @@
     <t>Building052</t>
   </si>
   <si>
-    <t>NameID_Item_Building052</t>
+    <t>NameID_Building052</t>
   </si>
   <si>
     <t>Item_Building060</t>
@@ -422,7 +422,7 @@
     <t>Building060</t>
   </si>
   <si>
-    <t>NameID_Item_Building060</t>
+    <t>NameID_Building060</t>
   </si>
   <si>
     <t>Item_Building061</t>
@@ -434,7 +434,7 @@
     <t>Building061</t>
   </si>
   <si>
-    <t>NameID_Item_Building061</t>
+    <t>NameID_Building061</t>
   </si>
   <si>
     <t>Item_Building062</t>
@@ -446,7 +446,7 @@
     <t>Building062</t>
   </si>
   <si>
-    <t>NameID_Item_Building062</t>
+    <t>NameID_Building062</t>
   </si>
   <si>
     <t>Item_Building070</t>
@@ -458,7 +458,7 @@
     <t>Building070</t>
   </si>
   <si>
-    <t>NameID_Item_Building070</t>
+    <t>NameID_Building070</t>
   </si>
   <si>
     <t>Item_Building071</t>
@@ -470,7 +470,7 @@
     <t>Building071</t>
   </si>
   <si>
-    <t>NameID_Item_Building071</t>
+    <t>NameID_Building071</t>
   </si>
   <si>
     <t>Item_Building072</t>
@@ -482,7 +482,7 @@
     <t>Building072</t>
   </si>
   <si>
-    <t>NameID_Item_Building072</t>
+    <t>NameID_Building072</t>
   </si>
   <si>
     <t>Item_Building080</t>
@@ -494,7 +494,7 @@
     <t>Building080</t>
   </si>
   <si>
-    <t>NameID_Item_Building080</t>
+    <t>NameID_Building080</t>
   </si>
   <si>
     <t>Item_Building081</t>
@@ -506,7 +506,7 @@
     <t>Building081</t>
   </si>
   <si>
-    <t>NameID_Item_Building081</t>
+    <t>NameID_Building081</t>
   </si>
   <si>
     <t>Item_Building082</t>
@@ -518,7 +518,7 @@
     <t>Building082</t>
   </si>
   <si>
-    <t>NameID_Item_Building082</t>
+    <t>NameID_Building082</t>
   </si>
   <si>
     <t>Item_Building090</t>
@@ -530,7 +530,7 @@
     <t>Building090</t>
   </si>
   <si>
-    <t>NameID_Item_Building090</t>
+    <t>NameID_Building090</t>
   </si>
   <si>
     <t>Item_Building091</t>
@@ -542,7 +542,7 @@
     <t>Building091</t>
   </si>
   <si>
-    <t>NameID_Item_Building091</t>
+    <t>NameID_Building091</t>
   </si>
   <si>
     <t>Item_Building092</t>
@@ -554,7 +554,7 @@
     <t>Building092</t>
   </si>
   <si>
-    <t>NameID_Item_Building092</t>
+    <t>NameID_Building092</t>
   </si>
   <si>
     <t>Item_Building100</t>
@@ -566,7 +566,7 @@
     <t>Building100</t>
   </si>
   <si>
-    <t>NameID_Item_Building100</t>
+    <t>NameID_Building100</t>
   </si>
   <si>
     <t>Item_Building101</t>
@@ -578,7 +578,7 @@
     <t>Building101</t>
   </si>
   <si>
-    <t>NameID_Item_Building101</t>
+    <t>NameID_Building101</t>
   </si>
   <si>
     <t>Item_Building102</t>
@@ -590,7 +590,7 @@
     <t>Building102</t>
   </si>
   <si>
-    <t>NameID_Item_Building102</t>
+    <t>NameID_Building102</t>
   </si>
   <si>
     <t>Item_Building110</t>
@@ -605,7 +605,7 @@
     <t>UIResources/BuildingSprite</t>
   </si>
   <si>
-    <t>NameID_Item_Building110</t>
+    <t>NameID_Building110</t>
   </si>
   <si>
     <t>Item_Building111</t>
@@ -617,7 +617,7 @@
     <t>Building111</t>
   </si>
   <si>
-    <t>NameID_Item_Building111</t>
+    <t>NameID_Building111</t>
   </si>
   <si>
     <t>Item_Building112</t>
@@ -629,7 +629,7 @@
     <t>Building112</t>
   </si>
   <si>
-    <t>NameID_Item_Building112</t>
+    <t>NameID_Building112</t>
   </si>
   <si>
     <t>Item_Building120</t>
@@ -641,7 +641,7 @@
     <t>Building120</t>
   </si>
   <si>
-    <t>NameID_Item_Building120</t>
+    <t>NameID_Building120</t>
   </si>
   <si>
     <t>Item_Building121</t>
@@ -653,7 +653,7 @@
     <t>Building121</t>
   </si>
   <si>
-    <t>NameID_Item_Building121</t>
+    <t>NameID_Building121</t>
   </si>
   <si>
     <t>Item_Building122</t>
@@ -665,7 +665,7 @@
     <t>Building122</t>
   </si>
   <si>
-    <t>NameID_Item_Building122</t>
+    <t>NameID_Building122</t>
   </si>
   <si>
     <t>Item_Building130</t>
@@ -677,7 +677,7 @@
     <t>Building130</t>
   </si>
   <si>
-    <t>NameID_Item_Building130</t>
+    <t>NameID_Building130</t>
   </si>
   <si>
     <t>Item_Building131</t>
@@ -689,7 +689,7 @@
     <t>Building131</t>
   </si>
   <si>
-    <t>NameID_Item_Building131</t>
+    <t>NameID_Building131</t>
   </si>
   <si>
     <t>Item_Building132</t>
@@ -701,7 +701,7 @@
     <t>Building132</t>
   </si>
   <si>
-    <t>NameID_Item_Building132</t>
+    <t>NameID_Building132</t>
   </si>
   <si>
     <t>Item_Building140</t>
@@ -713,7 +713,7 @@
     <t>Building140</t>
   </si>
   <si>
-    <t>NameID_Item_Building140</t>
+    <t>NameID_Building140</t>
   </si>
   <si>
     <t>Item_Building141</t>
@@ -725,7 +725,7 @@
     <t>Building141</t>
   </si>
   <si>
-    <t>NameID_Item_Building141</t>
+    <t>NameID_Building141</t>
   </si>
   <si>
     <t>Item_Building142</t>
@@ -737,7 +737,7 @@
     <t>Building142</t>
   </si>
   <si>
-    <t>NameID_Item_Building142</t>
+    <t>NameID_Building142</t>
   </si>
   <si>
     <t>Item_Building150</t>
@@ -749,7 +749,7 @@
     <t>Building150</t>
   </si>
   <si>
-    <t>NameID_Item_Building150</t>
+    <t>NameID_Building150</t>
   </si>
   <si>
     <t>Item_Building151</t>
@@ -761,7 +761,7 @@
     <t>Building151</t>
   </si>
   <si>
-    <t>NameID_Item_Building151</t>
+    <t>NameID_Building151</t>
   </si>
   <si>
     <t>Item_Building152</t>
@@ -773,7 +773,7 @@
     <t>Building152</t>
   </si>
   <si>
-    <t>NameID_Item_Building152</t>
+    <t>NameID_Building152</t>
   </si>
   <si>
     <t>Item_Building160</t>
@@ -785,7 +785,7 @@
     <t>Building160</t>
   </si>
   <si>
-    <t>NameID_Item_Building160</t>
+    <t>NameID_Building160</t>
   </si>
   <si>
     <t>Item_Building161</t>
@@ -797,7 +797,7 @@
     <t>Building161</t>
   </si>
   <si>
-    <t>NameID_Item_Building161</t>
+    <t>NameID_Building161</t>
   </si>
   <si>
     <t>Item_Building162</t>
@@ -809,7 +809,7 @@
     <t>Building162</t>
   </si>
   <si>
-    <t>NameID_Item_Building162</t>
+    <t>NameID_Building162</t>
   </si>
   <si>
     <t>Item_Building170</t>
@@ -821,7 +821,7 @@
     <t>Building170</t>
   </si>
   <si>
-    <t>NameID_Item_Building170</t>
+    <t>NameID_Building170</t>
   </si>
   <si>
     <t>Item_Building171</t>
@@ -833,7 +833,7 @@
     <t>Building171</t>
   </si>
   <si>
-    <t>NameID_Item_Building171</t>
+    <t>NameID_Building171</t>
   </si>
   <si>
     <t>Item_Building172</t>
@@ -845,7 +845,7 @@
     <t>Building172</t>
   </si>
   <si>
-    <t>NameID_Item_Building172</t>
+    <t>NameID_Building172</t>
   </si>
   <si>
     <t>Item_Building180</t>
@@ -857,7 +857,7 @@
     <t>Building180</t>
   </si>
   <si>
-    <t>NameID_Item_Building180</t>
+    <t>NameID_Building180</t>
   </si>
   <si>
     <t>Item_Building181</t>
@@ -869,7 +869,7 @@
     <t>Building181</t>
   </si>
   <si>
-    <t>NameID_Item_Building181</t>
+    <t>NameID_Building181</t>
   </si>
   <si>
     <t>Item_Building182</t>
@@ -881,7 +881,7 @@
     <t>Building182</t>
   </si>
   <si>
-    <t>NameID_Item_Building182</t>
+    <t>NameID_Building182</t>
   </si>
   <si>
     <t>Item_Building190</t>
@@ -893,7 +893,7 @@
     <t>Building190</t>
   </si>
   <si>
-    <t>NameID_Item_Building190</t>
+    <t>NameID_Building190</t>
   </si>
   <si>
     <t>Item_Building191</t>
@@ -905,7 +905,7 @@
     <t>Building191</t>
   </si>
   <si>
-    <t>NameID_Item_Building191</t>
+    <t>NameID_Building191</t>
   </si>
   <si>
     <t>Item_Building192</t>
@@ -917,7 +917,7 @@
     <t>Building192</t>
   </si>
   <si>
-    <t>NameID_Item_Building192</t>
+    <t>NameID_Building192</t>
   </si>
   <si>
     <t>Item_Building200</t>
@@ -929,7 +929,7 @@
     <t>Building200</t>
   </si>
   <si>
-    <t>NameID_Item_Building200</t>
+    <t>NameID_Building200</t>
   </si>
   <si>
     <t>Item_Building201</t>
@@ -941,7 +941,7 @@
     <t>Building201</t>
   </si>
   <si>
-    <t>NameID_Item_Building201</t>
+    <t>NameID_Building201</t>
   </si>
   <si>
     <t>Item_Building202</t>
@@ -953,7 +953,7 @@
     <t>Building202</t>
   </si>
   <si>
-    <t>NameID_Item_Building202</t>
+    <t>NameID_Building202</t>
   </si>
   <si>
     <t>Item_Gold_Item1</t>
@@ -1813,16 +1813,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1830,7 +1830,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1859,10 +1859,84 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1870,46 +1944,45 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1917,88 +1990,15 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -2060,25 +2060,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2090,7 +2102,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2108,7 +2150,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2120,7 +2162,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2132,13 +2186,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2150,37 +2216,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2192,49 +2228,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2399,6 +2399,44 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2414,11 +2452,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2452,197 +2496,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2716,10 +2716,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
@@ -2787,55 +2787,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -3118,44 +3118,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:V73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="Q11" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11:G73"/>
+      <selection pane="bottomRight" activeCell="U11" sqref="U11:U73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.3359375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="12.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="20.1666666666667" customWidth="1"/>
+    <col min="4" max="4" width="9.33333333333333" customWidth="1"/>
+    <col min="5" max="5" width="12.6666666666667" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.6666666666667" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="58.3359375" customWidth="1"/>
-    <col min="11" max="11" width="31.5078125" customWidth="1"/>
-    <col min="12" max="13" width="14.1640625" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="16.5078125" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="58.3333333333333" customWidth="1"/>
+    <col min="11" max="11" width="31.5083333333333" customWidth="1"/>
+    <col min="12" max="13" width="14.1666666666667" customWidth="1"/>
+    <col min="14" max="14" width="17.6666666666667" customWidth="1"/>
+    <col min="15" max="15" width="16.5083333333333" customWidth="1"/>
+    <col min="16" max="16" width="12.6666666666667" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
-    <col min="18" max="18" width="27.6640625" customWidth="1"/>
-    <col min="19" max="19" width="33.4296875" customWidth="1"/>
-    <col min="20" max="20" width="23.3359375" customWidth="1"/>
-    <col min="21" max="21" width="21.5078125" customWidth="1"/>
-    <col min="22" max="22" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="27.6666666666667" customWidth="1"/>
+    <col min="19" max="19" width="33.4333333333333" customWidth="1"/>
+    <col min="20" max="20" width="23.3333333333333" customWidth="1"/>
+    <col min="21" max="21" width="29.25" customWidth="1"/>
+    <col min="22" max="22" width="8.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:22">
+    <row r="1" s="1" customFormat="1" ht="27" spans="1:22">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="7" s="3" customFormat="1" spans="1:22">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="8" s="3" customFormat="1" spans="1:22">
       <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="9" s="3" customFormat="1" spans="1:22">
       <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="11" s="40" customFormat="1" spans="1:22">
       <c r="A11" s="41" t="s">
         <v>54</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="12" s="40" customFormat="1" spans="1:22">
       <c r="A12" s="41" t="s">
         <v>59</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="13" s="40" customFormat="1" spans="1:22">
       <c r="A13" s="41" t="s">
         <v>63</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="14" s="40" customFormat="1" spans="1:22">
       <c r="A14" s="42" t="s">
         <v>67</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="15" s="40" customFormat="1" spans="1:22">
       <c r="A15" s="42" t="s">
         <v>71</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="16" s="40" customFormat="1" spans="1:22">
       <c r="A16" s="42" t="s">
         <v>75</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="17" s="40" customFormat="1" spans="1:22">
       <c r="A17" s="42" t="s">
         <v>79</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="18" s="40" customFormat="1" spans="1:22">
       <c r="A18" s="42" t="s">
         <v>83</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="19" s="40" customFormat="1" spans="1:22">
       <c r="A19" s="42" t="s">
         <v>87</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="20" s="40" customFormat="1" spans="1:22">
       <c r="A20" s="42" t="s">
         <v>91</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="21" s="40" customFormat="1" spans="1:22">
       <c r="A21" s="42" t="s">
         <v>95</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="22" s="40" customFormat="1" spans="1:22">
       <c r="A22" s="42" t="s">
         <v>99</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="23" s="40" customFormat="1" spans="1:22">
       <c r="A23" s="42" t="s">
         <v>103</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="24" s="40" customFormat="1" spans="1:22">
       <c r="A24" s="42" t="s">
         <v>107</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="25" s="40" customFormat="1" spans="1:22">
       <c r="A25" s="42" t="s">
         <v>111</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="26" s="40" customFormat="1" spans="1:22">
       <c r="A26" s="42" t="s">
         <v>115</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="27" s="40" customFormat="1" spans="1:22">
       <c r="A27" s="42" t="s">
         <v>119</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="28" s="40" customFormat="1" spans="1:22">
       <c r="A28" s="42" t="s">
         <v>123</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="29" s="40" customFormat="1" spans="1:22">
       <c r="A29" s="42" t="s">
         <v>127</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="30" s="40" customFormat="1" spans="1:22">
       <c r="A30" s="42" t="s">
         <v>131</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" s="40" customFormat="1" ht="17" spans="1:22">
+    <row r="31" s="40" customFormat="1" spans="1:22">
       <c r="A31" s="42" t="s">
         <v>135</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="32" s="31" customFormat="1" spans="1:22">
       <c r="A32" s="42" t="s">
         <v>139</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="33" s="31" customFormat="1" spans="1:22">
       <c r="A33" s="42" t="s">
         <v>143</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="34" s="31" customFormat="1" spans="1:22">
       <c r="A34" s="42" t="s">
         <v>147</v>
       </c>
@@ -5227,7 +5227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="35" s="31" customFormat="1" spans="1:22">
       <c r="A35" s="42" t="s">
         <v>151</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="36" s="31" customFormat="1" spans="1:22">
       <c r="A36" s="42" t="s">
         <v>155</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="37" s="31" customFormat="1" spans="1:22">
       <c r="A37" s="42" t="s">
         <v>159</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="38" s="31" customFormat="1" spans="1:22">
       <c r="A38" s="42" t="s">
         <v>163</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="39" s="31" customFormat="1" spans="1:22">
       <c r="A39" s="42" t="s">
         <v>167</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="40" s="31" customFormat="1" spans="1:22">
       <c r="A40" s="42" t="s">
         <v>171</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="41" s="31" customFormat="1" spans="1:22">
       <c r="A41" s="42" t="s">
         <v>175</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="42" s="31" customFormat="1" spans="1:22">
       <c r="A42" s="42" t="s">
         <v>179</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="43" s="31" customFormat="1" spans="1:22">
       <c r="A43" s="42" t="s">
         <v>183</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="44" s="31" customFormat="1" spans="1:22">
       <c r="A44" s="42" t="s">
         <v>187</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="45" s="31" customFormat="1" spans="1:22">
       <c r="A45" s="42" t="s">
         <v>192</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="46" s="31" customFormat="1" spans="1:22">
       <c r="A46" s="42" t="s">
         <v>196</v>
       </c>
@@ -5923,7 +5923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="47" s="31" customFormat="1" spans="1:22">
       <c r="A47" s="42" t="s">
         <v>200</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="48" s="31" customFormat="1" spans="1:22">
       <c r="A48" s="42" t="s">
         <v>204</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="49" s="31" customFormat="1" spans="1:22">
       <c r="A49" s="42" t="s">
         <v>208</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="50" s="31" customFormat="1" spans="1:22">
       <c r="A50" s="42" t="s">
         <v>212</v>
       </c>
@@ -6155,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="51" s="31" customFormat="1" spans="1:22">
       <c r="A51" s="42" t="s">
         <v>216</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="52" s="31" customFormat="1" spans="1:22">
       <c r="A52" s="42" t="s">
         <v>220</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="53" s="31" customFormat="1" spans="1:22">
       <c r="A53" s="42" t="s">
         <v>224</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="54" s="31" customFormat="1" spans="1:22">
       <c r="A54" s="42" t="s">
         <v>228</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="55" s="31" customFormat="1" spans="1:22">
       <c r="A55" s="42" t="s">
         <v>232</v>
       </c>
@@ -6445,7 +6445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="56" s="31" customFormat="1" spans="1:22">
       <c r="A56" s="42" t="s">
         <v>236</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="57" s="31" customFormat="1" spans="1:22">
       <c r="A57" s="42" t="s">
         <v>240</v>
       </c>
@@ -6561,7 +6561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="58" s="31" customFormat="1" spans="1:22">
       <c r="A58" s="42" t="s">
         <v>244</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="59" s="31" customFormat="1" spans="1:22">
       <c r="A59" s="42" t="s">
         <v>248</v>
       </c>
@@ -6677,7 +6677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="60" s="31" customFormat="1" spans="1:22">
       <c r="A60" s="42" t="s">
         <v>252</v>
       </c>
@@ -6735,7 +6735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="61" s="31" customFormat="1" spans="1:22">
       <c r="A61" s="42" t="s">
         <v>256</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="62" s="31" customFormat="1" spans="1:22">
       <c r="A62" s="42" t="s">
         <v>260</v>
       </c>
@@ -6851,7 +6851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="63" s="31" customFormat="1" spans="1:22">
       <c r="A63" s="42" t="s">
         <v>264</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" s="31" customFormat="1" customHeight="1" spans="1:22">
+    <row r="64" s="31" customFormat="1" ht="14" customHeight="1" spans="1:22">
       <c r="A64" s="42" t="s">
         <v>268</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="65" s="31" customFormat="1" spans="1:22">
       <c r="A65" s="42" t="s">
         <v>272</v>
       </c>
@@ -7025,7 +7025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="66" s="31" customFormat="1" spans="1:22">
       <c r="A66" s="42" t="s">
         <v>276</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" s="31" customFormat="1" customHeight="1" spans="1:22">
+    <row r="67" s="31" customFormat="1" ht="14" customHeight="1" spans="1:22">
       <c r="A67" s="42" t="s">
         <v>280</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="68" s="31" customFormat="1" spans="1:22">
       <c r="A68" s="42" t="s">
         <v>284</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="69" s="31" customFormat="1" spans="1:22">
       <c r="A69" s="42" t="s">
         <v>288</v>
       </c>
@@ -7257,7 +7257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" s="31" customFormat="1" customHeight="1" spans="1:22">
+    <row r="70" s="31" customFormat="1" ht="14" customHeight="1" spans="1:22">
       <c r="A70" s="42" t="s">
         <v>292</v>
       </c>
@@ -7315,7 +7315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="71" s="31" customFormat="1" spans="1:22">
       <c r="A71" s="42" t="s">
         <v>296</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" s="31" customFormat="1" ht="17" spans="1:22">
+    <row r="72" s="31" customFormat="1" spans="1:22">
       <c r="A72" s="42" t="s">
         <v>300</v>
       </c>
@@ -7503,7 +7503,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:V49"/>
   <sheetViews>
@@ -7515,31 +7515,31 @@
       <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="30.2890625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.3359375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.2916666666667" customWidth="1"/>
+    <col min="2" max="2" width="12.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="20.1666666666667" customWidth="1"/>
+    <col min="4" max="4" width="9.33333333333333" customWidth="1"/>
+    <col min="5" max="5" width="12.6666666666667" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.6666666666667" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="58.3359375" customWidth="1"/>
-    <col min="11" max="11" width="31.5078125" customWidth="1"/>
-    <col min="12" max="13" width="14.1640625" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="16.5078125" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="58.3333333333333" customWidth="1"/>
+    <col min="11" max="11" width="31.5083333333333" customWidth="1"/>
+    <col min="12" max="13" width="14.1666666666667" customWidth="1"/>
+    <col min="14" max="14" width="17.6666666666667" customWidth="1"/>
+    <col min="15" max="15" width="16.5083333333333" customWidth="1"/>
+    <col min="16" max="16" width="12.6666666666667" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
-    <col min="18" max="18" width="27.6640625" customWidth="1"/>
-    <col min="19" max="20" width="23.3359375" customWidth="1"/>
-    <col min="21" max="21" width="21.5078125" customWidth="1"/>
-    <col min="22" max="22" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="27.6666666666667" customWidth="1"/>
+    <col min="19" max="20" width="23.3333333333333" customWidth="1"/>
+    <col min="21" max="21" width="21.5083333333333" customWidth="1"/>
+    <col min="22" max="22" width="8.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:22">
+    <row r="1" s="1" customFormat="1" ht="27" spans="1:22">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7947,7 +7947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="7" s="3" customFormat="1" spans="1:22">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="8" s="3" customFormat="1" spans="1:22">
       <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
@@ -8083,7 +8083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="9" s="3" customFormat="1" spans="1:22">
       <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
@@ -10429,7 +10429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:V29"/>
   <sheetViews>
@@ -10441,28 +10441,28 @@
       <selection pane="bottomRight" activeCell="U11" sqref="U11:U29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.3359375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="12.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="20.1666666666667" customWidth="1"/>
+    <col min="4" max="4" width="9.33333333333333" customWidth="1"/>
+    <col min="5" max="5" width="12.6666666666667" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.6666666666667" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="58.3359375" customWidth="1"/>
-    <col min="11" max="11" width="31.5078125" customWidth="1"/>
-    <col min="12" max="13" width="14.1640625" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="16.5078125" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="58.3333333333333" customWidth="1"/>
+    <col min="11" max="11" width="31.5083333333333" customWidth="1"/>
+    <col min="12" max="13" width="14.1666666666667" customWidth="1"/>
+    <col min="14" max="14" width="17.6666666666667" customWidth="1"/>
+    <col min="15" max="15" width="16.5083333333333" customWidth="1"/>
+    <col min="16" max="16" width="12.6666666666667" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
-    <col min="18" max="18" width="27.6640625" customWidth="1"/>
-    <col min="19" max="20" width="23.3359375" customWidth="1"/>
-    <col min="21" max="21" width="21.5078125" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" customWidth="1"/>
+    <col min="18" max="18" width="27.6666666666667" customWidth="1"/>
+    <col min="19" max="20" width="23.3333333333333" customWidth="1"/>
+    <col min="21" max="21" width="21.5083333333333" customWidth="1"/>
+    <col min="22" max="22" width="10.5666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:22">
@@ -10873,7 +10873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="7" s="3" customFormat="1" spans="1:22">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -10941,7 +10941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="8" s="3" customFormat="1" spans="1:22">
       <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
@@ -11009,7 +11009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="9" s="3" customFormat="1" spans="1:22">
       <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
@@ -11145,7 +11145,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" s="20" customFormat="1" ht="17.55" spans="1:22">
+    <row r="11" s="20" customFormat="1" ht="14.25" spans="1:22">
       <c r="A11" s="21" t="s">
         <v>402</v>
       </c>
@@ -11162,7 +11162,7 @@
       <c r="F11" s="22">
         <v>0</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="23" t="s">
         <v>403</v>
       </c>
       <c r="H11" s="22"/>
@@ -11203,48 +11203,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" s="20" customFormat="1" ht="17.55" spans="1:22">
+    <row r="12" s="20" customFormat="1" ht="14.25" spans="1:22">
       <c r="A12" s="21" t="s">
         <v>407</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="24">
         <v>3</v>
       </c>
-      <c r="C12" s="23">
-        <v>0</v>
-      </c>
-      <c r="D12" s="23">
-        <v>0</v>
-      </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23">
-        <v>0</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="C12" s="24">
+        <v>0</v>
+      </c>
+      <c r="D12" s="24">
+        <v>0</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24">
+        <v>0</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="26"/>
-      <c r="K12" s="23">
-        <v>0</v>
-      </c>
-      <c r="L12" s="23">
-        <v>0</v>
-      </c>
-      <c r="M12" s="23">
-        <v>1</v>
-      </c>
-      <c r="N12" s="23">
+      <c r="K12" s="24">
+        <v>0</v>
+      </c>
+      <c r="L12" s="24">
+        <v>0</v>
+      </c>
+      <c r="M12" s="24">
+        <v>1</v>
+      </c>
+      <c r="N12" s="24">
         <v>0</v>
       </c>
       <c r="O12" s="22">
         <v>1000</v>
       </c>
-      <c r="P12" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="23"/>
+      <c r="P12" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="24"/>
       <c r="R12" s="27" t="s">
         <v>409</v>
       </c>
@@ -11257,11 +11257,11 @@
       <c r="U12" s="30" t="s">
         <v>410</v>
       </c>
-      <c r="V12" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" s="20" customFormat="1" ht="17.55" spans="1:22">
+      <c r="V12" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" s="20" customFormat="1" ht="14.25" spans="1:22">
       <c r="A13" s="21" t="s">
         <v>411</v>
       </c>
@@ -11271,38 +11271,38 @@
       <c r="C13" s="22">
         <v>0</v>
       </c>
-      <c r="D13" s="23">
-        <v>0</v>
-      </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23">
-        <v>0</v>
-      </c>
-      <c r="G13" s="24" t="s">
+      <c r="D13" s="24">
+        <v>0</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24">
+        <v>0</v>
+      </c>
+      <c r="G13" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
       <c r="J13" s="26"/>
-      <c r="K13" s="23">
-        <v>0</v>
-      </c>
-      <c r="L13" s="23">
-        <v>0</v>
-      </c>
-      <c r="M13" s="23">
-        <v>1</v>
-      </c>
-      <c r="N13" s="23">
+      <c r="K13" s="24">
+        <v>0</v>
+      </c>
+      <c r="L13" s="24">
+        <v>0</v>
+      </c>
+      <c r="M13" s="24">
+        <v>1</v>
+      </c>
+      <c r="N13" s="24">
         <v>0</v>
       </c>
       <c r="O13" s="22">
         <v>1000</v>
       </c>
-      <c r="P13" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="23"/>
+      <c r="P13" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="24"/>
       <c r="R13" s="27" t="s">
         <v>413</v>
       </c>
@@ -11315,52 +11315,52 @@
       <c r="U13" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="V13" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" s="20" customFormat="1" ht="17.55" spans="1:22">
+      <c r="V13" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" s="20" customFormat="1" ht="14.25" spans="1:22">
       <c r="A14" s="21" t="s">
         <v>415</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="24">
         <v>3</v>
       </c>
-      <c r="C14" s="23">
-        <v>0</v>
-      </c>
-      <c r="D14" s="23">
-        <v>0</v>
-      </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23">
-        <v>0</v>
-      </c>
-      <c r="G14" s="24" t="s">
+      <c r="C14" s="24">
+        <v>0</v>
+      </c>
+      <c r="D14" s="24">
+        <v>0</v>
+      </c>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24">
+        <v>0</v>
+      </c>
+      <c r="G14" s="23" t="s">
         <v>416</v>
       </c>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="26"/>
-      <c r="K14" s="23">
-        <v>0</v>
-      </c>
-      <c r="L14" s="23">
-        <v>0</v>
-      </c>
-      <c r="M14" s="23">
-        <v>1</v>
-      </c>
-      <c r="N14" s="23">
+      <c r="K14" s="24">
+        <v>0</v>
+      </c>
+      <c r="L14" s="24">
+        <v>0</v>
+      </c>
+      <c r="M14" s="24">
+        <v>1</v>
+      </c>
+      <c r="N14" s="24">
         <v>0</v>
       </c>
       <c r="O14" s="22">
         <v>1000</v>
       </c>
-      <c r="P14" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="23"/>
+      <c r="P14" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="24"/>
       <c r="R14" s="27" t="s">
         <v>417</v>
       </c>
@@ -11373,11 +11373,11 @@
       <c r="U14" s="30" t="s">
         <v>418</v>
       </c>
-      <c r="V14" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" ht="17.55" spans="1:22">
+      <c r="V14" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" spans="1:22">
       <c r="A15" s="21" t="s">
         <v>419</v>
       </c>
@@ -11394,7 +11394,7 @@
       <c r="F15" s="22">
         <v>0</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="23" t="s">
         <v>420</v>
       </c>
       <c r="H15" s="22"/>
@@ -11435,48 +11435,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" ht="17.55" spans="1:22">
+    <row r="16" ht="14.25" spans="1:22">
       <c r="A16" s="21" t="s">
         <v>423</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="24">
         <v>3</v>
       </c>
-      <c r="C16" s="23">
-        <v>0</v>
-      </c>
-      <c r="D16" s="23">
-        <v>0</v>
-      </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23">
-        <v>0</v>
-      </c>
-      <c r="G16" s="24" t="s">
+      <c r="C16" s="24">
+        <v>0</v>
+      </c>
+      <c r="D16" s="24">
+        <v>0</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24">
+        <v>0</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>424</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="26"/>
-      <c r="K16" s="23">
-        <v>0</v>
-      </c>
-      <c r="L16" s="23">
-        <v>0</v>
-      </c>
-      <c r="M16" s="23">
-        <v>1</v>
-      </c>
-      <c r="N16" s="23">
+      <c r="K16" s="24">
+        <v>0</v>
+      </c>
+      <c r="L16" s="24">
+        <v>0</v>
+      </c>
+      <c r="M16" s="24">
+        <v>1</v>
+      </c>
+      <c r="N16" s="24">
         <v>0</v>
       </c>
       <c r="O16" s="22">
         <v>1000</v>
       </c>
-      <c r="P16" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="23"/>
+      <c r="P16" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="24"/>
       <c r="R16" s="27" t="s">
         <v>425</v>
       </c>
@@ -11489,11 +11489,11 @@
       <c r="U16" s="30" t="s">
         <v>426</v>
       </c>
-      <c r="V16" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" ht="17.55" spans="1:22">
+      <c r="V16" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" spans="1:22">
       <c r="A17" s="21" t="s">
         <v>427</v>
       </c>
@@ -11503,38 +11503,38 @@
       <c r="C17" s="22">
         <v>0</v>
       </c>
-      <c r="D17" s="23">
-        <v>0</v>
-      </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23">
-        <v>0</v>
-      </c>
-      <c r="G17" s="24" t="s">
+      <c r="D17" s="24">
+        <v>0</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24">
+        <v>0</v>
+      </c>
+      <c r="G17" s="23" t="s">
         <v>428</v>
       </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="26"/>
-      <c r="K17" s="23">
-        <v>0</v>
-      </c>
-      <c r="L17" s="23">
-        <v>0</v>
-      </c>
-      <c r="M17" s="23">
-        <v>1</v>
-      </c>
-      <c r="N17" s="23">
+      <c r="K17" s="24">
+        <v>0</v>
+      </c>
+      <c r="L17" s="24">
+        <v>0</v>
+      </c>
+      <c r="M17" s="24">
+        <v>1</v>
+      </c>
+      <c r="N17" s="24">
         <v>0</v>
       </c>
       <c r="O17" s="22">
         <v>1000</v>
       </c>
-      <c r="P17" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="23"/>
+      <c r="P17" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="24"/>
       <c r="R17" s="27" t="s">
         <v>429</v>
       </c>
@@ -11547,52 +11547,52 @@
       <c r="U17" s="30" t="s">
         <v>430</v>
       </c>
-      <c r="V17" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" ht="17.55" spans="1:22">
+      <c r="V17" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" spans="1:22">
       <c r="A18" s="21" t="s">
         <v>431</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="24">
         <v>3</v>
       </c>
-      <c r="C18" s="23">
-        <v>0</v>
-      </c>
-      <c r="D18" s="23">
-        <v>0</v>
-      </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23">
-        <v>0</v>
-      </c>
-      <c r="G18" s="24" t="s">
+      <c r="C18" s="24">
+        <v>0</v>
+      </c>
+      <c r="D18" s="24">
+        <v>0</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24">
+        <v>0</v>
+      </c>
+      <c r="G18" s="23" t="s">
         <v>432</v>
       </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
       <c r="J18" s="26"/>
-      <c r="K18" s="23">
-        <v>0</v>
-      </c>
-      <c r="L18" s="23">
-        <v>0</v>
-      </c>
-      <c r="M18" s="23">
-        <v>1</v>
-      </c>
-      <c r="N18" s="23">
+      <c r="K18" s="24">
+        <v>0</v>
+      </c>
+      <c r="L18" s="24">
+        <v>0</v>
+      </c>
+      <c r="M18" s="24">
+        <v>1</v>
+      </c>
+      <c r="N18" s="24">
         <v>0</v>
       </c>
       <c r="O18" s="22">
         <v>1000</v>
       </c>
-      <c r="P18" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="23"/>
+      <c r="P18" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="24"/>
       <c r="R18" s="27" t="s">
         <v>433</v>
       </c>
@@ -11605,11 +11605,11 @@
       <c r="U18" s="30" t="s">
         <v>434</v>
       </c>
-      <c r="V18" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" ht="17.55" spans="1:22">
+      <c r="V18" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" spans="1:22">
       <c r="A19" s="21" t="s">
         <v>435</v>
       </c>
@@ -11626,7 +11626,7 @@
       <c r="F19" s="22">
         <v>0</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="23" t="s">
         <v>436</v>
       </c>
       <c r="H19" s="22"/>
@@ -11667,48 +11667,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" ht="17.55" spans="1:22">
+    <row r="20" ht="14.25" spans="1:22">
       <c r="A20" s="21" t="s">
         <v>439</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="24">
         <v>3</v>
       </c>
-      <c r="C20" s="23">
-        <v>0</v>
-      </c>
-      <c r="D20" s="23">
-        <v>0</v>
-      </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23">
-        <v>0</v>
-      </c>
-      <c r="G20" s="24" t="s">
+      <c r="C20" s="24">
+        <v>0</v>
+      </c>
+      <c r="D20" s="24">
+        <v>0</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24">
+        <v>0</v>
+      </c>
+      <c r="G20" s="23" t="s">
         <v>440</v>
       </c>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
       <c r="J20" s="26"/>
-      <c r="K20" s="23">
-        <v>0</v>
-      </c>
-      <c r="L20" s="23">
-        <v>0</v>
-      </c>
-      <c r="M20" s="23">
-        <v>1</v>
-      </c>
-      <c r="N20" s="23">
+      <c r="K20" s="24">
+        <v>0</v>
+      </c>
+      <c r="L20" s="24">
+        <v>0</v>
+      </c>
+      <c r="M20" s="24">
+        <v>1</v>
+      </c>
+      <c r="N20" s="24">
         <v>0</v>
       </c>
       <c r="O20" s="22">
         <v>1000</v>
       </c>
-      <c r="P20" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="23"/>
+      <c r="P20" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="24"/>
       <c r="R20" s="27" t="s">
         <v>441</v>
       </c>
@@ -11721,11 +11721,11 @@
       <c r="U20" s="30" t="s">
         <v>442</v>
       </c>
-      <c r="V20" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" ht="17.55" spans="1:22">
+      <c r="V20" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" spans="1:22">
       <c r="A21" s="21" t="s">
         <v>443</v>
       </c>
@@ -11735,38 +11735,38 @@
       <c r="C21" s="22">
         <v>0</v>
       </c>
-      <c r="D21" s="23">
-        <v>0</v>
-      </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23">
-        <v>0</v>
-      </c>
-      <c r="G21" s="24" t="s">
+      <c r="D21" s="24">
+        <v>0</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24">
+        <v>0</v>
+      </c>
+      <c r="G21" s="23" t="s">
         <v>444</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="26"/>
-      <c r="K21" s="23">
-        <v>0</v>
-      </c>
-      <c r="L21" s="23">
-        <v>0</v>
-      </c>
-      <c r="M21" s="23">
-        <v>1</v>
-      </c>
-      <c r="N21" s="23">
+      <c r="K21" s="24">
+        <v>0</v>
+      </c>
+      <c r="L21" s="24">
+        <v>0</v>
+      </c>
+      <c r="M21" s="24">
+        <v>1</v>
+      </c>
+      <c r="N21" s="24">
         <v>0</v>
       </c>
       <c r="O21" s="22">
         <v>1000</v>
       </c>
-      <c r="P21" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="23"/>
+      <c r="P21" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="24"/>
       <c r="R21" s="27" t="s">
         <v>445</v>
       </c>
@@ -11779,52 +11779,52 @@
       <c r="U21" s="30" t="s">
         <v>446</v>
       </c>
-      <c r="V21" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" ht="17.55" spans="1:22">
+      <c r="V21" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" spans="1:22">
       <c r="A22" s="21" t="s">
         <v>447</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="24">
         <v>3</v>
       </c>
-      <c r="C22" s="23">
-        <v>0</v>
-      </c>
-      <c r="D22" s="23">
-        <v>0</v>
-      </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23">
-        <v>0</v>
-      </c>
-      <c r="G22" s="24" t="s">
+      <c r="C22" s="24">
+        <v>0</v>
+      </c>
+      <c r="D22" s="24">
+        <v>0</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24">
+        <v>0</v>
+      </c>
+      <c r="G22" s="23" t="s">
         <v>448</v>
       </c>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="26"/>
-      <c r="K22" s="23">
-        <v>0</v>
-      </c>
-      <c r="L22" s="23">
-        <v>0</v>
-      </c>
-      <c r="M22" s="23">
-        <v>1</v>
-      </c>
-      <c r="N22" s="23">
+      <c r="K22" s="24">
+        <v>0</v>
+      </c>
+      <c r="L22" s="24">
+        <v>0</v>
+      </c>
+      <c r="M22" s="24">
+        <v>1</v>
+      </c>
+      <c r="N22" s="24">
         <v>0</v>
       </c>
       <c r="O22" s="22">
         <v>1000</v>
       </c>
-      <c r="P22" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="23"/>
+      <c r="P22" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="24"/>
       <c r="R22" s="27" t="s">
         <v>449</v>
       </c>
@@ -11837,11 +11837,11 @@
       <c r="U22" s="30" t="s">
         <v>450</v>
       </c>
-      <c r="V22" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" ht="17.55" spans="1:22">
+      <c r="V22" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" spans="1:22">
       <c r="A23" s="21" t="s">
         <v>451</v>
       </c>
@@ -11858,7 +11858,7 @@
       <c r="F23" s="22">
         <v>0</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="23" t="s">
         <v>452</v>
       </c>
       <c r="H23" s="22"/>
@@ -11899,48 +11899,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" ht="17.55" spans="1:22">
+    <row r="24" ht="14.25" spans="1:22">
       <c r="A24" s="21" t="s">
         <v>455</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="24">
         <v>3</v>
       </c>
-      <c r="C24" s="23">
-        <v>0</v>
-      </c>
-      <c r="D24" s="23">
-        <v>0</v>
-      </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23">
-        <v>0</v>
-      </c>
-      <c r="G24" s="24" t="s">
+      <c r="C24" s="24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="23" t="s">
         <v>456</v>
       </c>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="26"/>
-      <c r="K24" s="23">
-        <v>0</v>
-      </c>
-      <c r="L24" s="23">
-        <v>0</v>
-      </c>
-      <c r="M24" s="23">
-        <v>1</v>
-      </c>
-      <c r="N24" s="23">
+      <c r="K24" s="24">
+        <v>0</v>
+      </c>
+      <c r="L24" s="24">
+        <v>0</v>
+      </c>
+      <c r="M24" s="24">
+        <v>1</v>
+      </c>
+      <c r="N24" s="24">
         <v>0</v>
       </c>
       <c r="O24" s="22">
         <v>1000</v>
       </c>
-      <c r="P24" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="23"/>
+      <c r="P24" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="24"/>
       <c r="R24" s="27" t="s">
         <v>457</v>
       </c>
@@ -11953,11 +11953,11 @@
       <c r="U24" s="30" t="s">
         <v>458</v>
       </c>
-      <c r="V24" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" ht="17.55" spans="1:22">
+      <c r="V24" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" spans="1:22">
       <c r="A25" s="21" t="s">
         <v>459</v>
       </c>
@@ -11967,38 +11967,38 @@
       <c r="C25" s="22">
         <v>0</v>
       </c>
-      <c r="D25" s="23">
-        <v>0</v>
-      </c>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23">
-        <v>0</v>
-      </c>
-      <c r="G25" s="24" t="s">
+      <c r="D25" s="24">
+        <v>0</v>
+      </c>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24">
+        <v>0</v>
+      </c>
+      <c r="G25" s="23" t="s">
         <v>460</v>
       </c>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="26"/>
-      <c r="K25" s="23">
-        <v>0</v>
-      </c>
-      <c r="L25" s="23">
-        <v>0</v>
-      </c>
-      <c r="M25" s="23">
-        <v>1</v>
-      </c>
-      <c r="N25" s="23">
+      <c r="K25" s="24">
+        <v>0</v>
+      </c>
+      <c r="L25" s="24">
+        <v>0</v>
+      </c>
+      <c r="M25" s="24">
+        <v>1</v>
+      </c>
+      <c r="N25" s="24">
         <v>0</v>
       </c>
       <c r="O25" s="22">
         <v>1000</v>
       </c>
-      <c r="P25" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="23"/>
+      <c r="P25" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="24"/>
       <c r="R25" s="27" t="s">
         <v>461</v>
       </c>
@@ -12011,52 +12011,52 @@
       <c r="U25" s="30" t="s">
         <v>462</v>
       </c>
-      <c r="V25" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" ht="17.55" spans="1:22">
+      <c r="V25" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" spans="1:22">
       <c r="A26" s="21" t="s">
         <v>463</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="24">
         <v>3</v>
       </c>
-      <c r="C26" s="23">
-        <v>0</v>
-      </c>
-      <c r="D26" s="23">
-        <v>0</v>
-      </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23">
-        <v>0</v>
-      </c>
-      <c r="G26" s="24" t="s">
+      <c r="C26" s="24">
+        <v>0</v>
+      </c>
+      <c r="D26" s="24">
+        <v>0</v>
+      </c>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24">
+        <v>0</v>
+      </c>
+      <c r="G26" s="23" t="s">
         <v>464</v>
       </c>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="26"/>
-      <c r="K26" s="23">
-        <v>0</v>
-      </c>
-      <c r="L26" s="23">
-        <v>0</v>
-      </c>
-      <c r="M26" s="23">
-        <v>1</v>
-      </c>
-      <c r="N26" s="23">
+      <c r="K26" s="24">
+        <v>0</v>
+      </c>
+      <c r="L26" s="24">
+        <v>0</v>
+      </c>
+      <c r="M26" s="24">
+        <v>1</v>
+      </c>
+      <c r="N26" s="24">
         <v>0</v>
       </c>
       <c r="O26" s="22">
         <v>1000</v>
       </c>
-      <c r="P26" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="23"/>
+      <c r="P26" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="24"/>
       <c r="R26" s="27" t="s">
         <v>465</v>
       </c>
@@ -12069,11 +12069,11 @@
       <c r="U26" s="30" t="s">
         <v>466</v>
       </c>
-      <c r="V26" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" ht="17.55" spans="1:22">
+      <c r="V26" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25" spans="1:22">
       <c r="A27" s="21" t="s">
         <v>467</v>
       </c>
@@ -12090,7 +12090,7 @@
       <c r="F27" s="22">
         <v>0</v>
       </c>
-      <c r="G27" s="24" t="s">
+      <c r="G27" s="23" t="s">
         <v>468</v>
       </c>
       <c r="H27" s="22"/>
@@ -12131,48 +12131,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" ht="17.55" spans="1:22">
+    <row r="28" ht="14.25" spans="1:22">
       <c r="A28" s="21" t="s">
         <v>471</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="24">
         <v>3</v>
       </c>
-      <c r="C28" s="23">
-        <v>0</v>
-      </c>
-      <c r="D28" s="23">
-        <v>0</v>
-      </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23">
-        <v>0</v>
-      </c>
-      <c r="G28" s="24" t="s">
+      <c r="C28" s="24">
+        <v>0</v>
+      </c>
+      <c r="D28" s="24">
+        <v>0</v>
+      </c>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24">
+        <v>0</v>
+      </c>
+      <c r="G28" s="23" t="s">
         <v>472</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
       <c r="J28" s="26"/>
-      <c r="K28" s="23">
-        <v>0</v>
-      </c>
-      <c r="L28" s="23">
-        <v>0</v>
-      </c>
-      <c r="M28" s="23">
-        <v>1</v>
-      </c>
-      <c r="N28" s="23">
+      <c r="K28" s="24">
+        <v>0</v>
+      </c>
+      <c r="L28" s="24">
+        <v>0</v>
+      </c>
+      <c r="M28" s="24">
+        <v>1</v>
+      </c>
+      <c r="N28" s="24">
         <v>0</v>
       </c>
       <c r="O28" s="22">
         <v>1000</v>
       </c>
-      <c r="P28" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="23"/>
+      <c r="P28" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="24"/>
       <c r="R28" s="27" t="s">
         <v>473</v>
       </c>
@@ -12185,11 +12185,11 @@
       <c r="U28" s="30" t="s">
         <v>474</v>
       </c>
-      <c r="V28" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" ht="16.8" spans="1:22">
+      <c r="V28" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="21" t="s">
         <v>475</v>
       </c>
@@ -12199,38 +12199,38 @@
       <c r="C29" s="22">
         <v>0</v>
       </c>
-      <c r="D29" s="23">
-        <v>0</v>
-      </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23">
-        <v>0</v>
-      </c>
-      <c r="G29" s="24" t="s">
+      <c r="D29" s="24">
+        <v>0</v>
+      </c>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24">
+        <v>0</v>
+      </c>
+      <c r="G29" s="23" t="s">
         <v>476</v>
       </c>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
       <c r="J29" s="26"/>
-      <c r="K29" s="23">
-        <v>0</v>
-      </c>
-      <c r="L29" s="23">
-        <v>0</v>
-      </c>
-      <c r="M29" s="23">
-        <v>1</v>
-      </c>
-      <c r="N29" s="23">
+      <c r="K29" s="24">
+        <v>0</v>
+      </c>
+      <c r="L29" s="24">
+        <v>0</v>
+      </c>
+      <c r="M29" s="24">
+        <v>1</v>
+      </c>
+      <c r="N29" s="24">
         <v>0</v>
       </c>
       <c r="O29" s="22">
         <v>1000</v>
       </c>
-      <c r="P29" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q29" s="23"/>
+      <c r="P29" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="24"/>
       <c r="R29" s="27" t="s">
         <v>477</v>
       </c>
@@ -12243,7 +12243,7 @@
       <c r="U29" s="30" t="s">
         <v>478</v>
       </c>
-      <c r="V29" s="23">
+      <c r="V29" s="24">
         <v>1</v>
       </c>
     </row>
@@ -12261,7 +12261,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:V26"/>
   <sheetViews>
@@ -12273,31 +12273,31 @@
       <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.3359375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="12.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="20.1666666666667" customWidth="1"/>
+    <col min="4" max="4" width="9.33333333333333" customWidth="1"/>
+    <col min="5" max="5" width="12.6666666666667" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.6666666666667" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="58.3359375" customWidth="1"/>
-    <col min="11" max="11" width="31.5078125" customWidth="1"/>
-    <col min="12" max="13" width="14.1640625" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="16.5078125" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="58.3333333333333" customWidth="1"/>
+    <col min="11" max="11" width="31.5083333333333" customWidth="1"/>
+    <col min="12" max="13" width="14.1666666666667" customWidth="1"/>
+    <col min="14" max="14" width="17.6666666666667" customWidth="1"/>
+    <col min="15" max="15" width="16.5083333333333" customWidth="1"/>
+    <col min="16" max="16" width="12.6666666666667" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
-    <col min="18" max="18" width="27.6640625" customWidth="1"/>
-    <col min="19" max="20" width="23.3359375" customWidth="1"/>
-    <col min="21" max="21" width="21.5078125" customWidth="1"/>
-    <col min="22" max="22" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="27.6666666666667" customWidth="1"/>
+    <col min="19" max="20" width="23.3333333333333" customWidth="1"/>
+    <col min="21" max="21" width="21.5083333333333" customWidth="1"/>
+    <col min="22" max="22" width="8.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:22">
+    <row r="1" s="1" customFormat="1" ht="27" spans="1:22">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -12705,7 +12705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="7" s="3" customFormat="1" spans="1:22">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -12773,7 +12773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="8" s="3" customFormat="1" spans="1:22">
       <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
@@ -12841,7 +12841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="9" s="3" customFormat="1" spans="1:22">
       <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
@@ -13887,7 +13887,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:V80"/>
   <sheetViews>
@@ -13899,31 +13899,31 @@
       <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.3359375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="12.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="20.1666666666667" customWidth="1"/>
+    <col min="4" max="4" width="9.33333333333333" customWidth="1"/>
+    <col min="5" max="5" width="12.6666666666667" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.6666666666667" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="58.3359375" customWidth="1"/>
-    <col min="11" max="11" width="31.5078125" customWidth="1"/>
-    <col min="12" max="13" width="14.1640625" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="16.5078125" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="58.3333333333333" customWidth="1"/>
+    <col min="11" max="11" width="31.5083333333333" customWidth="1"/>
+    <col min="12" max="13" width="14.1666666666667" customWidth="1"/>
+    <col min="14" max="14" width="17.6666666666667" customWidth="1"/>
+    <col min="15" max="15" width="16.5083333333333" customWidth="1"/>
+    <col min="16" max="16" width="12.6666666666667" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
-    <col min="18" max="18" width="27.6640625" customWidth="1"/>
-    <col min="19" max="20" width="23.3359375" customWidth="1"/>
-    <col min="21" max="21" width="21.5078125" customWidth="1"/>
-    <col min="22" max="22" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="27.6666666666667" customWidth="1"/>
+    <col min="19" max="20" width="23.3333333333333" customWidth="1"/>
+    <col min="21" max="21" width="21.5083333333333" customWidth="1"/>
+    <col min="22" max="22" width="8.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:22">
+    <row r="1" s="1" customFormat="1" ht="27" spans="1:22">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -14331,7 +14331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="7" s="3" customFormat="1" spans="1:22">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -14399,7 +14399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="8" s="3" customFormat="1" spans="1:22">
       <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
@@ -14467,7 +14467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="9" s="3" customFormat="1" spans="1:22">
       <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
@@ -18537,7 +18537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:V10"/>
   <sheetViews>
@@ -18549,31 +18549,31 @@
       <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.3359375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="12.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="20.1666666666667" customWidth="1"/>
+    <col min="4" max="4" width="9.33333333333333" customWidth="1"/>
+    <col min="5" max="5" width="12.6666666666667" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.6666666666667" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="58.3359375" customWidth="1"/>
-    <col min="11" max="11" width="31.5078125" customWidth="1"/>
-    <col min="12" max="13" width="14.1640625" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="16.5078125" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="58.3333333333333" customWidth="1"/>
+    <col min="11" max="11" width="31.5083333333333" customWidth="1"/>
+    <col min="12" max="13" width="14.1666666666667" customWidth="1"/>
+    <col min="14" max="14" width="17.6666666666667" customWidth="1"/>
+    <col min="15" max="15" width="16.5083333333333" customWidth="1"/>
+    <col min="16" max="16" width="12.6666666666667" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
-    <col min="18" max="18" width="27.6640625" customWidth="1"/>
-    <col min="19" max="20" width="23.3359375" customWidth="1"/>
-    <col min="21" max="21" width="21.5078125" customWidth="1"/>
-    <col min="22" max="22" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="27.6666666666667" customWidth="1"/>
+    <col min="19" max="20" width="23.3333333333333" customWidth="1"/>
+    <col min="21" max="21" width="21.5083333333333" customWidth="1"/>
+    <col min="22" max="22" width="8.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:22">
+    <row r="1" s="1" customFormat="1" ht="27" spans="1:22">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -18981,7 +18981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="7" s="3" customFormat="1" spans="1:22">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -19049,7 +19049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="8" s="3" customFormat="1" spans="1:22">
       <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
@@ -19117,7 +19117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" ht="17" spans="1:22">
+    <row r="9" s="3" customFormat="1" spans="1:22">
       <c r="A9" s="6" t="s">
         <v>32</v>
       </c>

</xml_diff>